<commit_message>
Test Product Summery Report Added
</commit_message>
<xml_diff>
--- a/Demo_Website_Testing/Test_Case_Design/Product_Test_Cases.xlsx
+++ b/Demo_Website_Testing/Test_Case_Design/Product_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wasana\University\Projects\QA-Portfolio\Demo_Website_Testing\Test_Case_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104BD611-F769-4C60-A9BF-6607901F7CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC1403B-F0A4-4A59-A41C-CDF8D3774237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>